<commit_message>
Final edits for trials
</commit_message>
<xml_diff>
--- a/data/London-Tets-Data.xlsx
+++ b/data/London-Tets-Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -44,15 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pressure Gradient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind Gradient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error</t>
   </si>
 </sst>
 </file>
@@ -63,11 +54,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -83,12 +75,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,15 +124,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,21 +149,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,18 +190,6 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -244,19 +217,6 @@
         <f aca="false">INT(F3-F2)</f>
         <v>-2</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <f aca="false">INT(J2-K2)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -284,19 +244,6 @@
         <f aca="false">INT(F4-F3)</f>
         <v>-4</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">INT(J3-K3)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -324,19 +271,6 @@
         <f aca="false">INT(F5-F4)</f>
         <v>-5</v>
       </c>
-      <c r="I4" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">INT(J4-K4)</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -364,19 +298,6 @@
         <f aca="false">INT(F6-F5)</f>
         <v>-4</v>
       </c>
-      <c r="I5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <f aca="false">INT(J5-K5)</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -404,19 +325,6 @@
         <f aca="false">INT(F7-F6)</f>
         <v>-5</v>
       </c>
-      <c r="I6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">INT(J6-K6)</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -444,19 +352,6 @@
         <f aca="false">INT(F8-F7)</f>
         <v>11</v>
       </c>
-      <c r="I7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <f aca="false">INT(J7-K7)</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -484,19 +379,6 @@
         <f aca="false">INT(F9-F8)</f>
         <v>7</v>
       </c>
-      <c r="I8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">INT(J8-K8)</f>
-        <v>3</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -524,19 +406,6 @@
         <f aca="false">INT(F10-F9)</f>
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <f aca="false">INT(J9-K9)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -564,19 +433,6 @@
         <f aca="false">INT(F11-F10)</f>
         <v>-4</v>
       </c>
-      <c r="I10" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <f aca="false">INT(J10-K10)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -604,19 +460,6 @@
         <f aca="false">INT(F12-F11)</f>
         <v>-2</v>
       </c>
-      <c r="I11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">INT(J11-K11)</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -644,19 +487,6 @@
         <f aca="false">INT(F13-F12)</f>
         <v>-4</v>
       </c>
-      <c r="I12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <f aca="false">INT(J12-K12)</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -684,19 +514,6 @@
         <f aca="false">INT(F14-F13)</f>
         <v>3</v>
       </c>
-      <c r="I13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">INT(J13-K13)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -724,19 +541,6 @@
         <f aca="false">INT(F15-F14)</f>
         <v>3</v>
       </c>
-      <c r="I14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">INT(J14-K14)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -764,19 +568,6 @@
         <f aca="false">INT(F16-F15)</f>
         <v>4</v>
       </c>
-      <c r="I15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">INT(J15-K15)</f>
-        <v>-1</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -804,19 +595,6 @@
         <f aca="false">INT(F17-F16)</f>
         <v>4</v>
       </c>
-      <c r="I16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">INT(J16-K16)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -844,19 +622,6 @@
         <f aca="false">INT(F18-F17)</f>
         <v>1</v>
       </c>
-      <c r="I17" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">INT(J17-K17)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -882,19 +647,6 @@
       </c>
       <c r="H18" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">INT(J18-K18)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>